<commit_message>
code modify to better understand
</commit_message>
<xml_diff>
--- a/Semana7Reto7/archivoExcel.xlsx
+++ b/Semana7Reto7/archivoExcel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,10 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>codigo</t>
+          <t>edad</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>carrera</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>costo</t>
         </is>
@@ -465,14 +460,9 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10000004</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Ingeniería de Alimentos</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+        <v>17</v>
+      </c>
+      <c r="D2" t="n">
         <v>5590000</v>
       </c>
     </row>
@@ -486,14 +476,9 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>10000006</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Contaduría Pública</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+        <v>18</v>
+      </c>
+      <c r="D3" t="n">
         <v>5431212</v>
       </c>
     </row>
@@ -507,14 +492,9 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>100000010</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Ingeniería Eléctrica</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+        <v>20</v>
+      </c>
+      <c r="D4" t="n">
         <v>5202121</v>
       </c>
     </row>

</xml_diff>